<commit_message>
change 2 excel manage scripts for caodixiong and wendy
</commit_message>
<xml_diff>
--- a/wendy/sample.xlsx
+++ b/wendy/sample.xlsx
@@ -15,129 +15,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
-  <si>
-    <t>9361289681090473650702</t>
-  </si>
-  <si>
-    <t>Fire 7 8GB</t>
-  </si>
-  <si>
-    <t>9361289681090473839763</t>
-  </si>
-  <si>
-    <t>1Z0W64A01352517131</t>
-  </si>
-  <si>
-    <t>9361289681090473759993</t>
-  </si>
-  <si>
-    <t>9361289681090473712509</t>
-  </si>
-  <si>
-    <t>9361289681090471972813</t>
-  </si>
-  <si>
-    <t>1ZY8A4000303130410</t>
-  </si>
-  <si>
-    <t>1Z9350XV0308337716</t>
-  </si>
-  <si>
-    <t>1Z9350YA0204194461</t>
-  </si>
-  <si>
-    <t>1Z9350YA0304179477</t>
-  </si>
-  <si>
-    <t>9361289681090481100480</t>
-  </si>
-  <si>
-    <t>1Z933E6V0360759395</t>
-  </si>
-  <si>
-    <t>1Z9350YA2904183977</t>
-  </si>
-  <si>
-    <t>1Z21F58E0361247124</t>
-  </si>
-  <si>
-    <t>TBA163541691000</t>
-  </si>
-  <si>
-    <t>9361289681090474253544</t>
-  </si>
-  <si>
-    <t>9361289681090474148413</t>
-  </si>
-  <si>
-    <t>1Z9350XV0308290847</t>
-  </si>
-  <si>
-    <t>1Z306AY10390247472</t>
-  </si>
-  <si>
-    <t>1Z2FX8251209978892</t>
-  </si>
-  <si>
-    <t>1ZR0951E0308323221</t>
-  </si>
-  <si>
-    <t>9361289681090472778384</t>
-  </si>
-  <si>
-    <t>9361289681090472778469</t>
-  </si>
-  <si>
-    <t>9361289681090473246400</t>
-  </si>
-  <si>
-    <t>9361289681090473312587</t>
-  </si>
-  <si>
-    <t>9361289681090472587290</t>
-  </si>
-  <si>
-    <t>9361289681090472764202</t>
-  </si>
-  <si>
-    <t>9361289681090473552440</t>
-  </si>
-  <si>
-    <t>9361289681090473970770</t>
-  </si>
-  <si>
-    <t>9361289681090474031722</t>
-  </si>
-  <si>
-    <t>1Z306AY10390542198</t>
-  </si>
-  <si>
-    <t>9361289681090473462992</t>
-  </si>
-  <si>
-    <t>1Z306AY10390708876</t>
-  </si>
-  <si>
-    <t>1Z377R950352582154</t>
-  </si>
-  <si>
-    <t>1Z9350XV0308317470</t>
-  </si>
-  <si>
-    <t>1Z9350XV0308318380</t>
-  </si>
-  <si>
-    <t>1Z147W7E0206106933</t>
-  </si>
-  <si>
-    <t>1Z933E6V0360116043</t>
-  </si>
-  <si>
-    <t>1Z306A400395107395</t>
-  </si>
-  <si>
-    <t>1Z9350XV0308334960</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+  <si>
+    <t>1ZW0184V0329692365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apple Watch Series 3 38mm </t>
+  </si>
+  <si>
+    <t>13256</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329693355</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329693373</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329693408</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329693293</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329693159</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689191</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329692516</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329692534</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329692570</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329692598</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689477</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689495</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689502</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689511</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689520</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689744</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689762</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689771</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689780</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689271</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689280</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689299</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689306</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329689315</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329690214</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329690223</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329690241</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329690278</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329690296</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329690876</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329690885</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329690894</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329690901</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329688754</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329688807</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329688843</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329688861</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329687273</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329687291</t>
+  </si>
+  <si>
+    <t>1ZW0184V0329687326</t>
   </si>
 </sst>
 </file>
@@ -473,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,22 +494,22 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="n">
-        <v>11344</v>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
-        <v>11344</v>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -511,13 +517,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="n">
-        <v>11344</v>
+      <c r="C3" t="s">
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -525,139 +531,139 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="n">
-        <v>11344</v>
+      <c r="C4" t="s">
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="n">
-        <v>11344</v>
+      <c r="C5" t="s">
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="n">
-        <v>11344</v>
+      <c r="C6" t="s">
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>11344</v>
+      <c r="C7" t="s">
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="n">
-        <v>721847988490</v>
+      <c r="A8" t="s">
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="n">
-        <v>11344</v>
+      <c r="C8" t="s">
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="n">
-        <v>11344</v>
+      <c r="C9" t="s">
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" t="n">
-        <v>11344</v>
+      <c r="C10" t="s">
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" t="n">
-        <v>11344</v>
+      <c r="C11" t="s">
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C12" t="n">
-        <v>11344</v>
+      <c r="C12" t="s">
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C13" t="n">
-        <v>11344</v>
+      <c r="C13" t="s">
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -665,27 +671,27 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="C14" t="n">
-        <v>11344</v>
+      <c r="C14" t="s">
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" t="n">
-        <v>11344</v>
+      <c r="C15" t="s">
+        <v>2</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -693,195 +699,195 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" t="n">
-        <v>11344</v>
+      <c r="C16" t="s">
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="n">
-        <v>11344</v>
+      <c r="C17" t="s">
+        <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C18" t="n">
-        <v>11344</v>
+      <c r="C18" t="s">
+        <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" t="n">
-        <v>11344</v>
+      <c r="C19" t="s">
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20" t="n">
-        <v>11344</v>
+      <c r="C20" t="s">
+        <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" t="n">
-        <v>11344</v>
+      <c r="C21" t="s">
+        <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="C22" t="n">
-        <v>11344</v>
+      <c r="C22" t="s">
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C23" t="n">
-        <v>11344</v>
+      <c r="C23" t="s">
+        <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
-      <c r="C24" t="n">
-        <v>11344</v>
+      <c r="C24" t="s">
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
-      <c r="C25" t="n">
-        <v>11344</v>
+      <c r="C25" t="s">
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C26" t="n">
-        <v>11344</v>
+      <c r="C26" t="s">
+        <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C27" t="n">
-        <v>11344</v>
+      <c r="C27" t="s">
+        <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
       </c>
-      <c r="C28" t="n">
-        <v>11344</v>
+      <c r="C28" t="s">
+        <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
-      <c r="C29" t="n">
-        <v>11344</v>
+      <c r="C29" t="s">
+        <v>2</v>
       </c>
       <c r="D29" t="n">
         <v>1</v>
@@ -889,13 +895,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
       </c>
-      <c r="C30" t="n">
-        <v>11344</v>
+      <c r="C30" t="s">
+        <v>2</v>
       </c>
       <c r="D30" t="n">
         <v>1</v>
@@ -903,69 +909,69 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="C31" t="n">
-        <v>11344</v>
+      <c r="C31" t="s">
+        <v>2</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="C32" t="n">
-        <v>11344</v>
+      <c r="C32" t="s">
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="C33" t="n">
-        <v>11344</v>
+      <c r="C33" t="s">
+        <v>2</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
-      <c r="C34" t="n">
-        <v>11344</v>
+      <c r="C34" t="s">
+        <v>2</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="C35" t="n">
-        <v>11344</v>
+      <c r="C35" t="s">
+        <v>2</v>
       </c>
       <c r="D35" t="n">
         <v>1</v>
@@ -973,146 +979,88 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
       </c>
-      <c r="C36" t="n">
-        <v>11344</v>
+      <c r="C36" t="s">
+        <v>2</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
-      <c r="C37" t="n">
-        <v>11344</v>
+      <c r="C37" t="s">
+        <v>2</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
-      <c r="C38" t="n">
-        <v>11344</v>
+      <c r="C38" t="s">
+        <v>2</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
       </c>
-      <c r="C39" t="n">
-        <v>11344</v>
+      <c r="C39" t="s">
+        <v>2</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
       </c>
-      <c r="C40" t="n">
-        <v>11344</v>
+      <c r="C40" t="s">
+        <v>2</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
       </c>
-      <c r="C41" t="n">
-        <v>11344</v>
+      <c r="C41" t="s">
+        <v>2</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4"/>
-    <row r="43" spans="1:4"/>
-    <row r="44" spans="1:4"/>
-    <row r="45" spans="1:4"/>
-    <row r="46" spans="1:4"/>
-    <row r="47" spans="1:4"/>
-    <row r="48" spans="1:4"/>
-    <row r="49" spans="1:4"/>
-    <row r="50" spans="1:4"/>
-    <row r="51" spans="1:4"/>
-    <row r="52" spans="1:4"/>
-    <row r="53" spans="1:4"/>
-    <row r="54" spans="1:4"/>
-    <row r="55" spans="1:4"/>
-    <row r="56" spans="1:4"/>
-    <row r="57" spans="1:4"/>
-    <row r="58" spans="1:4"/>
-    <row r="59" spans="1:4"/>
-    <row r="60" spans="1:4"/>
-    <row r="61" spans="1:4"/>
-    <row r="62" spans="1:4"/>
-    <row r="63" spans="1:4"/>
-    <row r="64" spans="1:4"/>
-    <row r="65" spans="1:4"/>
-    <row r="66" spans="1:4"/>
-    <row r="67" spans="1:4"/>
-    <row r="68" spans="1:4"/>
-    <row r="69" spans="1:4"/>
-    <row r="70" spans="1:4"/>
-    <row r="71" spans="1:4"/>
-    <row r="72" spans="1:4"/>
-    <row r="73" spans="1:4"/>
-    <row r="74" spans="1:4"/>
-    <row r="75" spans="1:4"/>
-    <row r="76" spans="1:4"/>
-    <row r="77" spans="1:4"/>
-    <row r="78" spans="1:4"/>
-    <row r="79" spans="1:4"/>
-    <row r="80" spans="1:4"/>
-    <row r="81" spans="1:4"/>
-    <row r="82" spans="1:4"/>
-    <row r="83" spans="1:4"/>
-    <row r="84" spans="1:4"/>
-    <row r="85" spans="1:4"/>
-    <row r="86" spans="1:4"/>
-    <row r="87" spans="1:4"/>
-    <row r="88" spans="1:4"/>
-    <row r="89" spans="1:4"/>
-    <row r="90" spans="1:4"/>
-    <row r="91" spans="1:4"/>
-    <row r="92" spans="1:4"/>
-    <row r="93" spans="1:4"/>
-    <row r="94" spans="1:4"/>
-    <row r="95" spans="1:4"/>
-    <row r="96" spans="1:4"/>
-    <row r="97" spans="1:4"/>
-    <row r="98" spans="1:4"/>
-    <row r="99" spans="1:4"/>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>